<commit_message>
added pin clasp to BOM, added CSV format
Basically just making it pretty
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brady\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brady\Documents\GitHub\EOH-Badge-2015\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="975" yWindow="0" windowWidth="23025" windowHeight="10320"/>
+    <workbookView xWindow="1980" yWindow="0" windowWidth="23025" windowHeight="10320"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
   <si>
     <t>SUPPLIER</t>
   </si>
@@ -111,6 +111,15 @@
   </si>
   <si>
     <t>Sum</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>Pin Clasp (Tie Tack)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Example </t>
   </si>
 </sst>
 </file>
@@ -173,10 +182,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -462,7 +472,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -697,13 +707,35 @@
         <v>210</v>
       </c>
     </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="3">
+        <f>5/12</f>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E12">
+        <v>350</v>
+      </c>
+      <c r="F12" s="3">
+        <f>E12*D12</f>
+        <v>145.83333333333334</v>
+      </c>
+    </row>
     <row r="14" spans="1:9" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H14" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I14" s="1">
-        <f>SUM(F2:F11)</f>
-        <v>1721.174</v>
+        <f>SUM(F2:F12)</f>
+        <v>1867.0073333333332</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -719,8 +751,9 @@
     <hyperlink ref="C9" r:id="rId8"/>
     <hyperlink ref="C10" r:id="rId9"/>
     <hyperlink ref="C11" r:id="rId10"/>
+    <hyperlink ref="C12" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>